<commit_message>
Updated wheel of fortune code for minor fixes and assessment plan completed
</commit_message>
<xml_diff>
--- a/Plans/Assessment_Plan.xlsx
+++ b/Plans/Assessment_Plan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4580EA3-9C38-4F07-BC3A-DB24F8D20A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78E8608-B2DC-475C-B973-A3248CA9BC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <t>Weekly Schedule Planner</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Ensure submitted by 9am</t>
+  </si>
+  <si>
+    <t>✖</t>
   </si>
 </sst>
 </file>
@@ -1042,6 +1045,134 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1070,141 +1201,13 @@
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -6235,8 +6238,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AP43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6340,45 +6343,45 @@
       <c r="AP2" s="29"/>
     </row>
     <row r="3" spans="1:42" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="51"/>
-      <c r="AE3" s="51"/>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="51"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="86"/>
+      <c r="AA3" s="86"/>
+      <c r="AB3" s="86"/>
+      <c r="AC3" s="86"/>
+      <c r="AD3" s="86"/>
+      <c r="AE3" s="86"/>
+      <c r="AF3" s="86"/>
+      <c r="AG3" s="86"/>
+      <c r="AH3" s="86"/>
+      <c r="AI3" s="86"/>
+      <c r="AJ3" s="86"/>
+      <c r="AK3" s="86"/>
+      <c r="AL3" s="86"/>
+      <c r="AM3" s="86"/>
     </row>
     <row r="4" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
@@ -6397,20 +6400,20 @@
       <c r="N4" s="17"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
-      <c r="Q4" s="73" t="s">
+      <c r="Q4" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="71">
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="77">
         <v>44792</v>
       </c>
-      <c r="W4" s="71"/>
-      <c r="X4" s="71"/>
-      <c r="Y4" s="71"/>
-      <c r="Z4" s="71"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
       <c r="AA4" s="13"/>
       <c r="AB4" s="13"/>
       <c r="AC4" s="13"/>
@@ -6475,49 +6478,49 @@
     <row r="6" spans="1:42" s="36" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="32"/>
       <c r="B6" s="33"/>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="54"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="89"/>
       <c r="N6" s="17"/>
       <c r="O6" s="13"/>
-      <c r="P6" s="52" t="s">
+      <c r="P6" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="53"/>
-      <c r="W6" s="53"/>
-      <c r="X6" s="53"/>
-      <c r="Y6" s="53"/>
-      <c r="Z6" s="54"/>
+      <c r="Q6" s="88"/>
+      <c r="R6" s="88"/>
+      <c r="S6" s="88"/>
+      <c r="T6" s="88"/>
+      <c r="U6" s="88"/>
+      <c r="V6" s="88"/>
+      <c r="W6" s="88"/>
+      <c r="X6" s="88"/>
+      <c r="Y6" s="88"/>
+      <c r="Z6" s="89"/>
       <c r="AA6" s="13"/>
       <c r="AB6" s="13"/>
-      <c r="AC6" s="52" t="s">
+      <c r="AC6" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="53"/>
-      <c r="AE6" s="53"/>
-      <c r="AF6" s="53"/>
-      <c r="AG6" s="53"/>
-      <c r="AH6" s="53"/>
-      <c r="AI6" s="53"/>
-      <c r="AJ6" s="53"/>
-      <c r="AK6" s="53"/>
-      <c r="AL6" s="53"/>
-      <c r="AM6" s="54"/>
+      <c r="AD6" s="88"/>
+      <c r="AE6" s="88"/>
+      <c r="AF6" s="88"/>
+      <c r="AG6" s="88"/>
+      <c r="AH6" s="88"/>
+      <c r="AI6" s="88"/>
+      <c r="AJ6" s="88"/>
+      <c r="AK6" s="88"/>
+      <c r="AL6" s="88"/>
+      <c r="AM6" s="89"/>
       <c r="AN6" s="34"/>
       <c r="AO6" s="35"/>
       <c r="AP6" s="35"/>
@@ -6525,43 +6528,43 @@
     <row r="7" spans="1:42" s="24" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="83"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="55"/>
       <c r="N7" s="22"/>
       <c r="O7" s="23"/>
       <c r="P7" s="7"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
-      <c r="U7" s="59"/>
-      <c r="V7" s="59"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="59"/>
-      <c r="Y7" s="59"/>
-      <c r="Z7" s="60"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="78"/>
+      <c r="S7" s="78"/>
+      <c r="T7" s="78"/>
+      <c r="U7" s="78"/>
+      <c r="V7" s="78"/>
+      <c r="W7" s="78"/>
+      <c r="X7" s="78"/>
+      <c r="Y7" s="78"/>
+      <c r="Z7" s="79"/>
       <c r="AA7" s="23"/>
       <c r="AB7" s="23"/>
-      <c r="AC7" s="81"/>
-      <c r="AD7" s="82"/>
-      <c r="AE7" s="82"/>
-      <c r="AF7" s="82"/>
-      <c r="AG7" s="82"/>
-      <c r="AH7" s="82"/>
-      <c r="AI7" s="82"/>
-      <c r="AJ7" s="82"/>
-      <c r="AK7" s="82"/>
-      <c r="AL7" s="82"/>
-      <c r="AM7" s="83"/>
+      <c r="AC7" s="53"/>
+      <c r="AD7" s="54"/>
+      <c r="AE7" s="54"/>
+      <c r="AF7" s="54"/>
+      <c r="AG7" s="54"/>
+      <c r="AH7" s="54"/>
+      <c r="AI7" s="54"/>
+      <c r="AJ7" s="54"/>
+      <c r="AK7" s="54"/>
+      <c r="AL7" s="54"/>
+      <c r="AM7" s="55"/>
       <c r="AN7" s="21"/>
       <c r="AO7" s="20"/>
       <c r="AP7" s="20"/>
@@ -6569,43 +6572,43 @@
     <row r="8" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="58"/>
       <c r="N8" s="6"/>
       <c r="O8" s="5"/>
       <c r="P8" s="8"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
-      <c r="U8" s="62"/>
-      <c r="V8" s="62"/>
-      <c r="W8" s="62"/>
-      <c r="X8" s="62"/>
-      <c r="Y8" s="62"/>
-      <c r="Z8" s="63"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="66"/>
+      <c r="T8" s="66"/>
+      <c r="U8" s="66"/>
+      <c r="V8" s="66"/>
+      <c r="W8" s="66"/>
+      <c r="X8" s="66"/>
+      <c r="Y8" s="66"/>
+      <c r="Z8" s="67"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
-      <c r="AC8" s="84"/>
-      <c r="AD8" s="85"/>
-      <c r="AE8" s="85"/>
-      <c r="AF8" s="85"/>
-      <c r="AG8" s="85"/>
-      <c r="AH8" s="85"/>
-      <c r="AI8" s="85"/>
-      <c r="AJ8" s="85"/>
-      <c r="AK8" s="85"/>
-      <c r="AL8" s="85"/>
-      <c r="AM8" s="86"/>
+      <c r="AC8" s="56"/>
+      <c r="AD8" s="57"/>
+      <c r="AE8" s="57"/>
+      <c r="AF8" s="57"/>
+      <c r="AG8" s="57"/>
+      <c r="AH8" s="57"/>
+      <c r="AI8" s="57"/>
+      <c r="AJ8" s="57"/>
+      <c r="AK8" s="57"/>
+      <c r="AL8" s="57"/>
+      <c r="AM8" s="58"/>
       <c r="AN8" s="16"/>
       <c r="AO8" s="15"/>
       <c r="AP8" s="15"/>
@@ -6613,43 +6616,43 @@
     <row r="9" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="86"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="58"/>
       <c r="N9" s="6"/>
       <c r="O9" s="5"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="62"/>
-      <c r="W9" s="62"/>
-      <c r="X9" s="62"/>
-      <c r="Y9" s="62"/>
-      <c r="Z9" s="63"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="66"/>
+      <c r="T9" s="66"/>
+      <c r="U9" s="66"/>
+      <c r="V9" s="66"/>
+      <c r="W9" s="66"/>
+      <c r="X9" s="66"/>
+      <c r="Y9" s="66"/>
+      <c r="Z9" s="67"/>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
-      <c r="AC9" s="84"/>
-      <c r="AD9" s="85"/>
-      <c r="AE9" s="85"/>
-      <c r="AF9" s="85"/>
-      <c r="AG9" s="85"/>
-      <c r="AH9" s="85"/>
-      <c r="AI9" s="85"/>
-      <c r="AJ9" s="85"/>
-      <c r="AK9" s="85"/>
-      <c r="AL9" s="85"/>
-      <c r="AM9" s="86"/>
+      <c r="AC9" s="56"/>
+      <c r="AD9" s="57"/>
+      <c r="AE9" s="57"/>
+      <c r="AF9" s="57"/>
+      <c r="AG9" s="57"/>
+      <c r="AH9" s="57"/>
+      <c r="AI9" s="57"/>
+      <c r="AJ9" s="57"/>
+      <c r="AK9" s="57"/>
+      <c r="AL9" s="57"/>
+      <c r="AM9" s="58"/>
       <c r="AN9" s="16"/>
       <c r="AO9" s="15"/>
       <c r="AP9" s="15"/>
@@ -6657,43 +6660,43 @@
     <row r="10" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
-      <c r="H10" s="85"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="85"/>
-      <c r="M10" s="86"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="58"/>
       <c r="N10" s="6"/>
       <c r="O10" s="5"/>
       <c r="P10" s="8"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
-      <c r="T10" s="62"/>
-      <c r="U10" s="62"/>
-      <c r="V10" s="62"/>
-      <c r="W10" s="62"/>
-      <c r="X10" s="62"/>
-      <c r="Y10" s="62"/>
-      <c r="Z10" s="63"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
+      <c r="U10" s="66"/>
+      <c r="V10" s="66"/>
+      <c r="W10" s="66"/>
+      <c r="X10" s="66"/>
+      <c r="Y10" s="66"/>
+      <c r="Z10" s="67"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
-      <c r="AC10" s="84"/>
-      <c r="AD10" s="85"/>
-      <c r="AE10" s="85"/>
-      <c r="AF10" s="85"/>
-      <c r="AG10" s="85"/>
-      <c r="AH10" s="85"/>
-      <c r="AI10" s="85"/>
-      <c r="AJ10" s="85"/>
-      <c r="AK10" s="85"/>
-      <c r="AL10" s="85"/>
-      <c r="AM10" s="86"/>
+      <c r="AC10" s="56"/>
+      <c r="AD10" s="57"/>
+      <c r="AE10" s="57"/>
+      <c r="AF10" s="57"/>
+      <c r="AG10" s="57"/>
+      <c r="AH10" s="57"/>
+      <c r="AI10" s="57"/>
+      <c r="AJ10" s="57"/>
+      <c r="AK10" s="57"/>
+      <c r="AL10" s="57"/>
+      <c r="AM10" s="58"/>
       <c r="AN10" s="16"/>
       <c r="AO10" s="15"/>
       <c r="AP10" s="15"/>
@@ -6701,43 +6704,43 @@
     <row r="11" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="85"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="86"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="58"/>
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
       <c r="P11" s="8"/>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="62"/>
-      <c r="T11" s="62"/>
-      <c r="U11" s="62"/>
-      <c r="V11" s="62"/>
-      <c r="W11" s="62"/>
-      <c r="X11" s="62"/>
-      <c r="Y11" s="62"/>
-      <c r="Z11" s="63"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="66"/>
+      <c r="Z11" s="67"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
-      <c r="AC11" s="84"/>
-      <c r="AD11" s="85"/>
-      <c r="AE11" s="85"/>
-      <c r="AF11" s="85"/>
-      <c r="AG11" s="85"/>
-      <c r="AH11" s="85"/>
-      <c r="AI11" s="85"/>
-      <c r="AJ11" s="85"/>
-      <c r="AK11" s="85"/>
-      <c r="AL11" s="85"/>
-      <c r="AM11" s="86"/>
+      <c r="AC11" s="56"/>
+      <c r="AD11" s="57"/>
+      <c r="AE11" s="57"/>
+      <c r="AF11" s="57"/>
+      <c r="AG11" s="57"/>
+      <c r="AH11" s="57"/>
+      <c r="AI11" s="57"/>
+      <c r="AJ11" s="57"/>
+      <c r="AK11" s="57"/>
+      <c r="AL11" s="57"/>
+      <c r="AM11" s="58"/>
       <c r="AN11" s="16"/>
       <c r="AO11" s="15"/>
       <c r="AP11" s="15"/>
@@ -6745,43 +6748,43 @@
     <row r="12" spans="1:42" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="88"/>
-      <c r="M12" s="89"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="61"/>
       <c r="N12" s="6"/>
       <c r="O12" s="5"/>
       <c r="P12" s="9"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
-      <c r="U12" s="65"/>
-      <c r="V12" s="65"/>
-      <c r="W12" s="65"/>
-      <c r="X12" s="65"/>
-      <c r="Y12" s="65"/>
-      <c r="Z12" s="66"/>
+      <c r="Q12" s="68"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="68"/>
+      <c r="T12" s="68"/>
+      <c r="U12" s="68"/>
+      <c r="V12" s="68"/>
+      <c r="W12" s="68"/>
+      <c r="X12" s="68"/>
+      <c r="Y12" s="68"/>
+      <c r="Z12" s="69"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
-      <c r="AC12" s="87"/>
-      <c r="AD12" s="88"/>
-      <c r="AE12" s="88"/>
-      <c r="AF12" s="88"/>
-      <c r="AG12" s="88"/>
-      <c r="AH12" s="88"/>
-      <c r="AI12" s="88"/>
-      <c r="AJ12" s="88"/>
-      <c r="AK12" s="88"/>
-      <c r="AL12" s="88"/>
-      <c r="AM12" s="89"/>
+      <c r="AC12" s="59"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
+      <c r="AG12" s="60"/>
+      <c r="AH12" s="60"/>
+      <c r="AI12" s="60"/>
+      <c r="AJ12" s="60"/>
+      <c r="AK12" s="60"/>
+      <c r="AL12" s="60"/>
+      <c r="AM12" s="61"/>
       <c r="AN12" s="16"/>
       <c r="AO12" s="15"/>
       <c r="AP12" s="15"/>
@@ -6877,51 +6880,51 @@
     <row r="15" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="90" t="str">
+      <c r="C15" s="62" t="str">
         <f>TEXT(StartDate+0,"dd")</f>
         <v>19</v>
       </c>
-      <c r="D15" s="91"/>
-      <c r="E15" s="76" t="str">
+      <c r="D15" s="63"/>
+      <c r="E15" s="70" t="str">
         <f>(TEXT(StartDate+0,"aaaa"))</f>
         <v>Friday</v>
       </c>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="74" t="str">
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="81" t="str">
         <f>TEXT(StartDate+1,"dd")</f>
         <v>20</v>
       </c>
-      <c r="J15" s="74"/>
-      <c r="K15" s="76" t="str">
+      <c r="J15" s="81"/>
+      <c r="K15" s="70" t="str">
         <f>(TEXT(StartDate+1,"aaaa"))</f>
         <v>Saturday</v>
       </c>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="74" t="str">
+      <c r="L15" s="70"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="81" t="str">
         <f>TEXT(StartDate+2,"dd")</f>
         <v>21</v>
       </c>
-      <c r="O15" s="74"/>
-      <c r="P15" s="76" t="str">
+      <c r="O15" s="81"/>
+      <c r="P15" s="70" t="str">
         <f>(TEXT(StartDate+2,"aaaa"))</f>
         <v>Sunday</v>
       </c>
-      <c r="Q15" s="76"/>
-      <c r="R15" s="76"/>
-      <c r="S15" s="74" t="str">
+      <c r="Q15" s="70"/>
+      <c r="R15" s="70"/>
+      <c r="S15" s="81" t="str">
         <f>TEXT(StartDate+3,"dd")</f>
         <v>22</v>
       </c>
-      <c r="T15" s="74"/>
-      <c r="U15" s="76" t="str">
+      <c r="T15" s="81"/>
+      <c r="U15" s="70" t="str">
         <f>(TEXT(StartDate+3,"aaaa"))</f>
         <v>Monday</v>
       </c>
-      <c r="V15" s="76"/>
-      <c r="W15" s="76"/>
+      <c r="V15" s="70"/>
+      <c r="W15" s="70"/>
       <c r="X15" s="27"/>
       <c r="Y15" s="16"/>
       <c r="Z15" s="15"/>
@@ -6945,39 +6948,39 @@
     <row r="16" spans="1:42" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="77" t="str">
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="72" t="str">
         <f>(TEXT(StartDate+0,"mmmm"))</f>
         <v>August</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="77" t="str">
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="72" t="str">
         <f>(TEXT(StartDate+1,"mmmm"))</f>
         <v>August</v>
       </c>
-      <c r="L16" s="77"/>
-      <c r="M16" s="77"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="75"/>
-      <c r="P16" s="77" t="str">
+      <c r="L16" s="72"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="82"/>
+      <c r="P16" s="72" t="str">
         <f>(TEXT(StartDate+2,"mmmm"))</f>
         <v>August</v>
       </c>
-      <c r="Q16" s="77"/>
-      <c r="R16" s="77"/>
-      <c r="S16" s="75"/>
-      <c r="T16" s="75"/>
-      <c r="U16" s="77" t="str">
+      <c r="Q16" s="72"/>
+      <c r="R16" s="72"/>
+      <c r="S16" s="82"/>
+      <c r="T16" s="82"/>
+      <c r="U16" s="72" t="str">
         <f>(TEXT(StartDate+3,"mmmm"))</f>
         <v>August</v>
       </c>
-      <c r="V16" s="77"/>
-      <c r="W16" s="77"/>
+      <c r="V16" s="72"/>
+      <c r="W16" s="72"/>
       <c r="X16" s="28"/>
       <c r="Y16" s="16"/>
       <c r="Z16" s="15"/>
@@ -7004,38 +7007,40 @@
       <c r="C17" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="D17" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
       <c r="I17" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="68" t="s">
+      <c r="J17" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="68"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
       <c r="N17" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="O17" s="68" t="s">
+      <c r="O17" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="P17" s="68"/>
-      <c r="Q17" s="68"/>
-      <c r="R17" s="68"/>
-      <c r="S17" s="46"/>
-      <c r="T17" s="68" t="s">
+      <c r="P17" s="74"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="T17" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="U17" s="68"/>
-      <c r="V17" s="68"/>
-      <c r="W17" s="68"/>
+      <c r="U17" s="74"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="74"/>
       <c r="X17" s="41"/>
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
@@ -7062,36 +7067,40 @@
       <c r="C18" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="69" t="s">
+      <c r="D18" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="72"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="76"/>
       <c r="I18" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="69" t="s">
+      <c r="J18" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="69" t="s">
+      <c r="K18" s="75"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="47"/>
-      <c r="T18" s="69" t="s">
+      <c r="P18" s="75"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="T18" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-      <c r="W18" s="69"/>
+      <c r="U18" s="75"/>
+      <c r="V18" s="75"/>
+      <c r="W18" s="75"/>
       <c r="X18" s="43"/>
       <c r="Y18" s="16"/>
       <c r="Z18" s="15"/>
@@ -7118,34 +7127,36 @@
       <c r="C19" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="69" t="s">
+      <c r="D19" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="72"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="76"/>
       <c r="I19" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="69" t="s">
+      <c r="J19" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="69" t="s">
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="O19" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="69"/>
-      <c r="R19" s="72"/>
+      <c r="P19" s="75"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="76"/>
       <c r="S19" s="47"/>
-      <c r="T19" s="69"/>
-      <c r="U19" s="69"/>
-      <c r="V19" s="69"/>
-      <c r="W19" s="72"/>
+      <c r="T19" s="75"/>
+      <c r="U19" s="75"/>
+      <c r="V19" s="75"/>
+      <c r="W19" s="76"/>
       <c r="X19" s="43"/>
       <c r="Y19" s="16"/>
       <c r="Z19" s="15"/>
@@ -7172,36 +7183,36 @@
       <c r="C20" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="69" t="s">
+      <c r="D20" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="72"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="76"/>
       <c r="I20" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J20" s="69" t="s">
+      <c r="J20" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
       <c r="N20" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="O20" s="69" t="s">
+      <c r="O20" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
-      <c r="R20" s="69"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="75"/>
       <c r="S20" s="47"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="69"/>
-      <c r="W20" s="69"/>
+      <c r="T20" s="75"/>
+      <c r="U20" s="75"/>
+      <c r="V20" s="75"/>
+      <c r="W20" s="75"/>
       <c r="X20" s="43"/>
       <c r="Y20" s="16"/>
       <c r="Z20" s="15"/>
@@ -7228,32 +7239,36 @@
       <c r="C21" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="69" t="s">
+      <c r="D21" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="69" t="s">
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="69" t="s">
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
+      <c r="M21" s="75"/>
+      <c r="N21" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="O21" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="69"/>
-      <c r="R21" s="69"/>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
       <c r="S21" s="47"/>
-      <c r="T21" s="69"/>
-      <c r="U21" s="69"/>
-      <c r="V21" s="69"/>
-      <c r="W21" s="69"/>
+      <c r="T21" s="75"/>
+      <c r="U21" s="75"/>
+      <c r="V21" s="75"/>
+      <c r="W21" s="75"/>
       <c r="X21" s="43"/>
       <c r="Y21" s="16"/>
       <c r="Z21" s="15"/>
@@ -7280,34 +7295,36 @@
       <c r="C22" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="69" t="s">
+      <c r="D22" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="72"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="76"/>
       <c r="I22" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="69" t="s">
+      <c r="J22" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="69"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="69"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="69" t="s">
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="P22" s="69"/>
-      <c r="Q22" s="69"/>
-      <c r="R22" s="69"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
       <c r="S22" s="47"/>
-      <c r="T22" s="69"/>
-      <c r="U22" s="69"/>
-      <c r="V22" s="69"/>
-      <c r="W22" s="69"/>
+      <c r="T22" s="75"/>
+      <c r="U22" s="75"/>
+      <c r="V22" s="75"/>
+      <c r="W22" s="75"/>
       <c r="X22" s="43"/>
       <c r="Y22" s="16"/>
       <c r="Z22" s="15"/>
@@ -7334,34 +7351,36 @@
       <c r="C23" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="69" t="s">
+      <c r="D23" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="69" t="s">
+      <c r="J23" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="69" t="s">
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="P23" s="69"/>
-      <c r="Q23" s="69"/>
-      <c r="R23" s="69"/>
+      <c r="P23" s="75"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="75"/>
       <c r="S23" s="47"/>
-      <c r="T23" s="69"/>
-      <c r="U23" s="69"/>
-      <c r="V23" s="69"/>
-      <c r="W23" s="69"/>
+      <c r="T23" s="75"/>
+      <c r="U23" s="75"/>
+      <c r="V23" s="75"/>
+      <c r="W23" s="75"/>
       <c r="X23" s="43"/>
       <c r="Y23" s="16"/>
       <c r="Z23" s="15"/>
@@ -7386,30 +7405,32 @@
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="49"/>
-      <c r="D24" s="69" t="s">
+      <c r="D24" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
       <c r="I24" s="47"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="69" t="s">
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="O24" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="P24" s="69"/>
-      <c r="Q24" s="69"/>
-      <c r="R24" s="69"/>
+      <c r="P24" s="75"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="75"/>
       <c r="S24" s="47"/>
-      <c r="T24" s="69"/>
-      <c r="U24" s="69"/>
-      <c r="V24" s="69"/>
-      <c r="W24" s="69"/>
+      <c r="T24" s="75"/>
+      <c r="U24" s="75"/>
+      <c r="V24" s="75"/>
+      <c r="W24" s="75"/>
       <c r="X24" s="43"/>
       <c r="Y24" s="16"/>
       <c r="Z24" s="15"/>
@@ -7436,28 +7457,28 @@
       <c r="C25" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="69" t="s">
+      <c r="D25" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
       <c r="I25" s="47"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="75"/>
+      <c r="M25" s="75"/>
       <c r="N25" s="47"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
-      <c r="Q25" s="69"/>
-      <c r="R25" s="69"/>
+      <c r="O25" s="75"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="75"/>
       <c r="S25" s="47"/>
-      <c r="T25" s="69"/>
-      <c r="U25" s="69"/>
-      <c r="V25" s="69"/>
-      <c r="W25" s="69"/>
+      <c r="T25" s="75"/>
+      <c r="U25" s="75"/>
+      <c r="V25" s="75"/>
+      <c r="W25" s="75"/>
       <c r="X25" s="43"/>
       <c r="Y25" s="16"/>
       <c r="Z25" s="15"/>
@@ -7482,26 +7503,26 @@
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="42"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
       <c r="I26" s="47"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
       <c r="N26" s="47"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="69"/>
-      <c r="Q26" s="69"/>
-      <c r="R26" s="69"/>
+      <c r="O26" s="75"/>
+      <c r="P26" s="75"/>
+      <c r="Q26" s="75"/>
+      <c r="R26" s="75"/>
       <c r="S26" s="47"/>
-      <c r="T26" s="69"/>
-      <c r="U26" s="69"/>
-      <c r="V26" s="69"/>
-      <c r="W26" s="69"/>
+      <c r="T26" s="75"/>
+      <c r="U26" s="75"/>
+      <c r="V26" s="75"/>
+      <c r="W26" s="75"/>
       <c r="X26" s="43"/>
       <c r="Y26" s="16"/>
       <c r="Z26" s="15"/>
@@ -7526,26 +7547,26 @@
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="42"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
       <c r="I27" s="47"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
-      <c r="M27" s="69"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
       <c r="N27" s="47"/>
-      <c r="O27" s="69"/>
-      <c r="P27" s="69"/>
-      <c r="Q27" s="69"/>
-      <c r="R27" s="69"/>
+      <c r="O27" s="75"/>
+      <c r="P27" s="75"/>
+      <c r="Q27" s="75"/>
+      <c r="R27" s="75"/>
       <c r="S27" s="47"/>
-      <c r="T27" s="69"/>
-      <c r="U27" s="69"/>
-      <c r="V27" s="69"/>
-      <c r="W27" s="69"/>
+      <c r="T27" s="75"/>
+      <c r="U27" s="75"/>
+      <c r="V27" s="75"/>
+      <c r="W27" s="75"/>
       <c r="X27" s="43"/>
       <c r="Y27" s="16"/>
       <c r="Z27" s="15"/>
@@ -7570,26 +7591,26 @@
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="42"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
       <c r="I28" s="47"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="75"/>
       <c r="N28" s="47"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
-      <c r="Q28" s="69"/>
-      <c r="R28" s="69"/>
+      <c r="O28" s="75"/>
+      <c r="P28" s="75"/>
+      <c r="Q28" s="75"/>
+      <c r="R28" s="75"/>
       <c r="S28" s="47"/>
-      <c r="T28" s="69"/>
-      <c r="U28" s="69"/>
-      <c r="V28" s="69"/>
-      <c r="W28" s="69"/>
+      <c r="T28" s="75"/>
+      <c r="U28" s="75"/>
+      <c r="V28" s="75"/>
+      <c r="W28" s="75"/>
       <c r="X28" s="43"/>
       <c r="Y28" s="16"/>
       <c r="Z28" s="15"/>
@@ -7614,26 +7635,26 @@
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="42"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
       <c r="I29" s="47"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
+      <c r="M29" s="75"/>
       <c r="N29" s="47"/>
-      <c r="O29" s="69"/>
-      <c r="P29" s="69"/>
-      <c r="Q29" s="69"/>
-      <c r="R29" s="69"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="75"/>
       <c r="S29" s="47"/>
-      <c r="T29" s="69"/>
-      <c r="U29" s="69"/>
-      <c r="V29" s="69"/>
-      <c r="W29" s="69"/>
+      <c r="T29" s="75"/>
+      <c r="U29" s="75"/>
+      <c r="V29" s="75"/>
+      <c r="W29" s="75"/>
       <c r="X29" s="43"/>
       <c r="Y29" s="16"/>
       <c r="Z29" s="15"/>
@@ -7658,26 +7679,26 @@
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="42"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
       <c r="I30" s="47"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
+      <c r="M30" s="75"/>
       <c r="N30" s="47"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="69"/>
-      <c r="R30" s="69"/>
+      <c r="O30" s="75"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="75"/>
       <c r="S30" s="47"/>
-      <c r="T30" s="69"/>
-      <c r="U30" s="69"/>
-      <c r="V30" s="69"/>
-      <c r="W30" s="69"/>
+      <c r="T30" s="75"/>
+      <c r="U30" s="75"/>
+      <c r="V30" s="75"/>
+      <c r="W30" s="75"/>
       <c r="X30" s="43"/>
       <c r="Y30" s="16"/>
       <c r="Z30" s="15"/>
@@ -7702,26 +7723,26 @@
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="42"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="70"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
       <c r="I31" s="43"/>
-      <c r="J31" s="70"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="70"/>
-      <c r="M31" s="70"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="83"/>
+      <c r="L31" s="83"/>
+      <c r="M31" s="83"/>
       <c r="N31" s="43"/>
-      <c r="O31" s="70"/>
-      <c r="P31" s="70"/>
-      <c r="Q31" s="70"/>
-      <c r="R31" s="70"/>
+      <c r="O31" s="83"/>
+      <c r="P31" s="83"/>
+      <c r="Q31" s="83"/>
+      <c r="R31" s="83"/>
       <c r="S31" s="43"/>
-      <c r="T31" s="70"/>
-      <c r="U31" s="70"/>
-      <c r="V31" s="70"/>
-      <c r="W31" s="70"/>
+      <c r="T31" s="83"/>
+      <c r="U31" s="83"/>
+      <c r="V31" s="83"/>
+      <c r="W31" s="83"/>
       <c r="X31" s="43"/>
       <c r="Y31" s="16"/>
       <c r="Z31" s="15"/>
@@ -7746,26 +7767,26 @@
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="44"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="84"/>
       <c r="I32" s="45"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="67"/>
+      <c r="J32" s="84"/>
+      <c r="K32" s="84"/>
+      <c r="L32" s="84"/>
+      <c r="M32" s="84"/>
       <c r="N32" s="45"/>
-      <c r="O32" s="67"/>
-      <c r="P32" s="67"/>
-      <c r="Q32" s="67"/>
-      <c r="R32" s="67"/>
+      <c r="O32" s="84"/>
+      <c r="P32" s="84"/>
+      <c r="Q32" s="84"/>
+      <c r="R32" s="84"/>
       <c r="S32" s="45"/>
-      <c r="T32" s="67"/>
-      <c r="U32" s="67"/>
-      <c r="V32" s="67"/>
-      <c r="W32" s="67"/>
+      <c r="T32" s="84"/>
+      <c r="U32" s="84"/>
+      <c r="V32" s="84"/>
+      <c r="W32" s="84"/>
       <c r="X32" s="45"/>
       <c r="Y32" s="16"/>
       <c r="Z32" s="15"/>
@@ -7877,45 +7898,45 @@
     <row r="35" spans="1:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="11"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="55" t="s">
+      <c r="C35" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="56"/>
-      <c r="S35" s="56"/>
-      <c r="T35" s="56"/>
-      <c r="U35" s="56"/>
-      <c r="V35" s="56"/>
-      <c r="W35" s="56"/>
-      <c r="X35" s="56"/>
-      <c r="Y35" s="56"/>
-      <c r="Z35" s="56"/>
-      <c r="AA35" s="56"/>
-      <c r="AB35" s="56"/>
-      <c r="AC35" s="56"/>
-      <c r="AD35" s="56"/>
-      <c r="AE35" s="56"/>
-      <c r="AF35" s="56"/>
-      <c r="AG35" s="56"/>
-      <c r="AH35" s="56"/>
-      <c r="AI35" s="56"/>
-      <c r="AJ35" s="56"/>
-      <c r="AK35" s="56"/>
-      <c r="AL35" s="56"/>
-      <c r="AM35" s="57"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="91"/>
+      <c r="G35" s="91"/>
+      <c r="H35" s="91"/>
+      <c r="I35" s="91"/>
+      <c r="J35" s="91"/>
+      <c r="K35" s="91"/>
+      <c r="L35" s="91"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="91"/>
+      <c r="O35" s="91"/>
+      <c r="P35" s="91"/>
+      <c r="Q35" s="91"/>
+      <c r="R35" s="91"/>
+      <c r="S35" s="91"/>
+      <c r="T35" s="91"/>
+      <c r="U35" s="91"/>
+      <c r="V35" s="91"/>
+      <c r="W35" s="91"/>
+      <c r="X35" s="91"/>
+      <c r="Y35" s="91"/>
+      <c r="Z35" s="91"/>
+      <c r="AA35" s="91"/>
+      <c r="AB35" s="91"/>
+      <c r="AC35" s="91"/>
+      <c r="AD35" s="91"/>
+      <c r="AE35" s="91"/>
+      <c r="AF35" s="91"/>
+      <c r="AG35" s="91"/>
+      <c r="AH35" s="91"/>
+      <c r="AI35" s="91"/>
+      <c r="AJ35" s="91"/>
+      <c r="AK35" s="91"/>
+      <c r="AL35" s="91"/>
+      <c r="AM35" s="92"/>
       <c r="AN35" s="16"/>
       <c r="AO35" s="15"/>
       <c r="AP35" s="15"/>
@@ -7923,43 +7944,43 @@
     <row r="36" spans="1:42" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="25"/>
       <c r="B36" s="26"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59"/>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="59"/>
-      <c r="S36" s="59"/>
-      <c r="T36" s="59"/>
-      <c r="U36" s="59"/>
-      <c r="V36" s="59"/>
-      <c r="W36" s="59"/>
-      <c r="X36" s="59"/>
-      <c r="Y36" s="59"/>
-      <c r="Z36" s="59"/>
-      <c r="AA36" s="59"/>
-      <c r="AB36" s="59"/>
-      <c r="AC36" s="59"/>
-      <c r="AD36" s="59"/>
-      <c r="AE36" s="59"/>
-      <c r="AF36" s="59"/>
-      <c r="AG36" s="59"/>
-      <c r="AH36" s="59"/>
-      <c r="AI36" s="59"/>
-      <c r="AJ36" s="59"/>
-      <c r="AK36" s="59"/>
-      <c r="AL36" s="59"/>
-      <c r="AM36" s="60"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="78"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="78"/>
+      <c r="O36" s="78"/>
+      <c r="P36" s="78"/>
+      <c r="Q36" s="78"/>
+      <c r="R36" s="78"/>
+      <c r="S36" s="78"/>
+      <c r="T36" s="78"/>
+      <c r="U36" s="78"/>
+      <c r="V36" s="78"/>
+      <c r="W36" s="78"/>
+      <c r="X36" s="78"/>
+      <c r="Y36" s="78"/>
+      <c r="Z36" s="78"/>
+      <c r="AA36" s="78"/>
+      <c r="AB36" s="78"/>
+      <c r="AC36" s="78"/>
+      <c r="AD36" s="78"/>
+      <c r="AE36" s="78"/>
+      <c r="AF36" s="78"/>
+      <c r="AG36" s="78"/>
+      <c r="AH36" s="78"/>
+      <c r="AI36" s="78"/>
+      <c r="AJ36" s="78"/>
+      <c r="AK36" s="78"/>
+      <c r="AL36" s="78"/>
+      <c r="AM36" s="79"/>
       <c r="AN36" s="21"/>
       <c r="AO36" s="20"/>
       <c r="AP36" s="20"/>
@@ -7967,43 +7988,43 @@
     <row r="37" spans="1:42" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="25"/>
       <c r="B37" s="26"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
-      <c r="N37" s="79"/>
-      <c r="O37" s="79"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="79"/>
-      <c r="R37" s="79"/>
-      <c r="S37" s="79"/>
-      <c r="T37" s="79"/>
-      <c r="U37" s="79"/>
-      <c r="V37" s="79"/>
-      <c r="W37" s="79"/>
-      <c r="X37" s="79"/>
-      <c r="Y37" s="79"/>
-      <c r="Z37" s="79"/>
-      <c r="AA37" s="79"/>
-      <c r="AB37" s="79"/>
-      <c r="AC37" s="79"/>
-      <c r="AD37" s="79"/>
-      <c r="AE37" s="79"/>
-      <c r="AF37" s="79"/>
-      <c r="AG37" s="79"/>
-      <c r="AH37" s="79"/>
-      <c r="AI37" s="79"/>
-      <c r="AJ37" s="79"/>
-      <c r="AK37" s="79"/>
-      <c r="AL37" s="79"/>
-      <c r="AM37" s="80"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="51"/>
+      <c r="V37" s="51"/>
+      <c r="W37" s="51"/>
+      <c r="X37" s="51"/>
+      <c r="Y37" s="51"/>
+      <c r="Z37" s="51"/>
+      <c r="AA37" s="51"/>
+      <c r="AB37" s="51"/>
+      <c r="AC37" s="51"/>
+      <c r="AD37" s="51"/>
+      <c r="AE37" s="51"/>
+      <c r="AF37" s="51"/>
+      <c r="AG37" s="51"/>
+      <c r="AH37" s="51"/>
+      <c r="AI37" s="51"/>
+      <c r="AJ37" s="51"/>
+      <c r="AK37" s="51"/>
+      <c r="AL37" s="51"/>
+      <c r="AM37" s="52"/>
       <c r="AN37" s="21"/>
       <c r="AO37" s="20"/>
       <c r="AP37" s="20"/>
@@ -8011,43 +8032,43 @@
     <row r="38" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="62"/>
-      <c r="J38" s="62"/>
-      <c r="K38" s="62"/>
-      <c r="L38" s="62"/>
-      <c r="M38" s="62"/>
-      <c r="N38" s="62"/>
-      <c r="O38" s="62"/>
-      <c r="P38" s="62"/>
-      <c r="Q38" s="62"/>
-      <c r="R38" s="62"/>
-      <c r="S38" s="62"/>
-      <c r="T38" s="62"/>
-      <c r="U38" s="62"/>
-      <c r="V38" s="62"/>
-      <c r="W38" s="62"/>
-      <c r="X38" s="62"/>
-      <c r="Y38" s="62"/>
-      <c r="Z38" s="62"/>
-      <c r="AA38" s="62"/>
-      <c r="AB38" s="62"/>
-      <c r="AC38" s="62"/>
-      <c r="AD38" s="62"/>
-      <c r="AE38" s="62"/>
-      <c r="AF38" s="62"/>
-      <c r="AG38" s="62"/>
-      <c r="AH38" s="62"/>
-      <c r="AI38" s="62"/>
-      <c r="AJ38" s="62"/>
-      <c r="AK38" s="62"/>
-      <c r="AL38" s="62"/>
-      <c r="AM38" s="63"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
+      <c r="K38" s="66"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="66"/>
+      <c r="O38" s="66"/>
+      <c r="P38" s="66"/>
+      <c r="Q38" s="66"/>
+      <c r="R38" s="66"/>
+      <c r="S38" s="66"/>
+      <c r="T38" s="66"/>
+      <c r="U38" s="66"/>
+      <c r="V38" s="66"/>
+      <c r="W38" s="66"/>
+      <c r="X38" s="66"/>
+      <c r="Y38" s="66"/>
+      <c r="Z38" s="66"/>
+      <c r="AA38" s="66"/>
+      <c r="AB38" s="66"/>
+      <c r="AC38" s="66"/>
+      <c r="AD38" s="66"/>
+      <c r="AE38" s="66"/>
+      <c r="AF38" s="66"/>
+      <c r="AG38" s="66"/>
+      <c r="AH38" s="66"/>
+      <c r="AI38" s="66"/>
+      <c r="AJ38" s="66"/>
+      <c r="AK38" s="66"/>
+      <c r="AL38" s="66"/>
+      <c r="AM38" s="67"/>
       <c r="AN38" s="16"/>
       <c r="AO38" s="15"/>
       <c r="AP38" s="15"/>
@@ -8055,43 +8076,43 @@
     <row r="39" spans="1:42" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="11"/>
       <c r="B39" s="12"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="65"/>
-      <c r="K39" s="65"/>
-      <c r="L39" s="65"/>
-      <c r="M39" s="65"/>
-      <c r="N39" s="65"/>
-      <c r="O39" s="65"/>
-      <c r="P39" s="65"/>
-      <c r="Q39" s="65"/>
-      <c r="R39" s="65"/>
-      <c r="S39" s="65"/>
-      <c r="T39" s="65"/>
-      <c r="U39" s="65"/>
-      <c r="V39" s="65"/>
-      <c r="W39" s="65"/>
-      <c r="X39" s="65"/>
-      <c r="Y39" s="65"/>
-      <c r="Z39" s="65"/>
-      <c r="AA39" s="65"/>
-      <c r="AB39" s="65"/>
-      <c r="AC39" s="65"/>
-      <c r="AD39" s="65"/>
-      <c r="AE39" s="65"/>
-      <c r="AF39" s="65"/>
-      <c r="AG39" s="65"/>
-      <c r="AH39" s="65"/>
-      <c r="AI39" s="65"/>
-      <c r="AJ39" s="65"/>
-      <c r="AK39" s="65"/>
-      <c r="AL39" s="65"/>
-      <c r="AM39" s="66"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
+      <c r="N39" s="68"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="68"/>
+      <c r="Q39" s="68"/>
+      <c r="R39" s="68"/>
+      <c r="S39" s="68"/>
+      <c r="T39" s="68"/>
+      <c r="U39" s="68"/>
+      <c r="V39" s="68"/>
+      <c r="W39" s="68"/>
+      <c r="X39" s="68"/>
+      <c r="Y39" s="68"/>
+      <c r="Z39" s="68"/>
+      <c r="AA39" s="68"/>
+      <c r="AB39" s="68"/>
+      <c r="AC39" s="68"/>
+      <c r="AD39" s="68"/>
+      <c r="AE39" s="68"/>
+      <c r="AF39" s="68"/>
+      <c r="AG39" s="68"/>
+      <c r="AH39" s="68"/>
+      <c r="AI39" s="68"/>
+      <c r="AJ39" s="68"/>
+      <c r="AK39" s="68"/>
+      <c r="AL39" s="68"/>
+      <c r="AM39" s="69"/>
       <c r="AN39" s="16"/>
       <c r="AO39" s="15"/>
       <c r="AP39" s="15"/>
@@ -8229,6 +8250,87 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="105">
+    <mergeCell ref="C3:AM3"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="P6:Z6"/>
+    <mergeCell ref="AC6:AM6"/>
+    <mergeCell ref="C35:AM35"/>
+    <mergeCell ref="C36:AM36"/>
+    <mergeCell ref="C38:AM38"/>
+    <mergeCell ref="C39:AM39"/>
+    <mergeCell ref="O32:R32"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="T20:W20"/>
+    <mergeCell ref="T21:W21"/>
+    <mergeCell ref="T22:W22"/>
+    <mergeCell ref="T23:W23"/>
+    <mergeCell ref="T24:W24"/>
+    <mergeCell ref="T25:W25"/>
+    <mergeCell ref="T26:W26"/>
+    <mergeCell ref="T27:W27"/>
+    <mergeCell ref="T28:W28"/>
+    <mergeCell ref="T29:W29"/>
+    <mergeCell ref="T30:W30"/>
+    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="T32:W32"/>
+    <mergeCell ref="O28:R28"/>
+    <mergeCell ref="O29:R29"/>
+    <mergeCell ref="O30:R30"/>
+    <mergeCell ref="O31:R31"/>
+    <mergeCell ref="O26:R26"/>
+    <mergeCell ref="O27:R27"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O24:R24"/>
+    <mergeCell ref="O25:R25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="V4:Z4"/>
+    <mergeCell ref="Q7:Z7"/>
+    <mergeCell ref="Q8:Z8"/>
+    <mergeCell ref="Q9:Z9"/>
+    <mergeCell ref="Q10:Z10"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="T19:W19"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N15:O16"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="S15:T16"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="U16:W16"/>
     <mergeCell ref="C37:AM37"/>
     <mergeCell ref="C7:M7"/>
     <mergeCell ref="C8:M8"/>
@@ -8253,87 +8355,6 @@
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="D22:H22"/>
     <mergeCell ref="D23:H23"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="V4:Z4"/>
-    <mergeCell ref="Q7:Z7"/>
-    <mergeCell ref="Q8:Z8"/>
-    <mergeCell ref="Q9:Z9"/>
-    <mergeCell ref="Q10:Z10"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="T19:W19"/>
-    <mergeCell ref="Q4:U4"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N15:O16"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="S15:T16"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="O28:R28"/>
-    <mergeCell ref="O29:R29"/>
-    <mergeCell ref="O30:R30"/>
-    <mergeCell ref="O31:R31"/>
-    <mergeCell ref="O26:R26"/>
-    <mergeCell ref="O27:R27"/>
-    <mergeCell ref="O17:R17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="O24:R24"/>
-    <mergeCell ref="O25:R25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="C3:AM3"/>
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="P6:Z6"/>
-    <mergeCell ref="AC6:AM6"/>
-    <mergeCell ref="C35:AM35"/>
-    <mergeCell ref="C36:AM36"/>
-    <mergeCell ref="C38:AM38"/>
-    <mergeCell ref="C39:AM39"/>
-    <mergeCell ref="O32:R32"/>
-    <mergeCell ref="T17:W17"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="T20:W20"/>
-    <mergeCell ref="T21:W21"/>
-    <mergeCell ref="T22:W22"/>
-    <mergeCell ref="T23:W23"/>
-    <mergeCell ref="T24:W24"/>
-    <mergeCell ref="T25:W25"/>
-    <mergeCell ref="T26:W26"/>
-    <mergeCell ref="T27:W27"/>
-    <mergeCell ref="T28:W28"/>
-    <mergeCell ref="T29:W29"/>
-    <mergeCell ref="T30:W30"/>
-    <mergeCell ref="T31:W31"/>
-    <mergeCell ref="T32:W32"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:C12 C15 E15:E16 O13:AM13 C1:AM1 C17:D32 J17:J32 C36:C39 C44:AM1048576 C4:AM5 O6:O12 AA6:AB12">
     <cfRule type="cellIs" dxfId="58" priority="105" operator="equal">
@@ -8644,24 +8665,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="46e0ad8bcb937777a496f4378509b82b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3afd91b9dddacb5807afd727ccca0e2e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -8882,25 +8885,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D61C0559-A3A8-404B-B3C9-59977EEF143B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D895C161-5F30-4256-BAD3-309A58746C18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C3BEF7D-0560-4D92-8503-510D68BBABDD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8917,4 +8920,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D895C161-5F30-4256-BAD3-309A58746C18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D61C0559-A3A8-404B-B3C9-59977EEF143B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>